<commit_message>
Issu no.108 - Kolom M,N (SKP3) di takeout
</commit_message>
<xml_diff>
--- a/report/Custom Report - Personil Pendukung Pandu.xlsx
+++ b/report/Custom Report - Personil Pendukung Pandu.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947755EA-5BD3-422E-9810-331DA7AD95B9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PEND. PANDU" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>NO</t>
   </si>
@@ -45,15 +46,6 @@
     <t>CABANG</t>
   </si>
   <si>
-    <t>TANGGAL MULAI SK</t>
-  </si>
-  <si>
-    <t>TANGGAL MULAI SKPPP</t>
-  </si>
-  <si>
-    <t>TANGGAL SELESAI SKPPP</t>
-  </si>
-  <si>
     <t>${table:pk.nama}</t>
   </si>
   <si>
@@ -84,9 +76,6 @@
     <t>MANNING AGENCY</t>
   </si>
   <si>
-    <t>NO SK</t>
-  </si>
-  <si>
     <t>JENIS SERTIFIKAT</t>
   </si>
   <si>
@@ -111,12 +100,6 @@
     <t>${table:pk.TANGGAL_MULAI}</t>
   </si>
   <si>
-    <t>${table:pk.SKPP_TANGGAL_MULAI}</t>
-  </si>
-  <si>
-    <t>${table:pk.skpp_SKPP_TANGGAL_SELESAI}</t>
-  </si>
-  <si>
     <t>${table:pk.JENISCERT}</t>
   </si>
   <si>
@@ -139,12 +122,18 @@
   </si>
   <si>
     <t>${table:pk.KAPAL}</t>
+  </si>
+  <si>
+    <t>NO SK/PKL</t>
+  </si>
+  <si>
+    <t>TANGGAL MULAI SK/PKL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,45 +532,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.77734375" customWidth="1"/>
-    <col min="15" max="15" width="21.109375" customWidth="1"/>
-    <col min="16" max="16" width="34.77734375" customWidth="1"/>
-    <col min="17" max="17" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="22.44140625" customWidth="1"/>
-    <col min="33" max="33" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="34.7109375" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.42578125" customWidth="1"/>
+    <col min="31" max="31" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="3" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -607,113 +594,101 @@
         <v>4</v>
       </c>
       <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="G2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="N2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>